<commit_message>
Test: Add prime attribute test
</commit_message>
<xml_diff>
--- a/DC20Models.nUnitTests/Unit Tests/Character/BlackBox_Character.xlsx
+++ b/DC20Models.nUnitTests/Unit Tests/Character/BlackBox_Character.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Blazor\DC20 Character Sheet\TestGeneration\Character\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Blazor\DC20 Character Sheet\DC20Models\DC20Models.nUnitTests\Unit Tests\Character\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F87B90B-0597-4F57-A299-036CD78DFD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5502123-15FF-4004-9027-17F4CE4008B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14310" yWindow="0" windowWidth="14595" windowHeight="15585" activeTab="2" xr2:uid="{4151E963-BEFA-4E14-B0A5-BD998C18A418}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{4151E963-BEFA-4E14-B0A5-BD998C18A418}"/>
   </bookViews>
   <sheets>
     <sheet name="Constructor" sheetId="2" r:id="rId1"/>
     <sheet name="CombatMastery" sheetId="1" r:id="rId2"/>
     <sheet name="AttributeLimit" sheetId="3" r:id="rId3"/>
+    <sheet name="Prime" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
   <si>
     <t>Test Case</t>
   </si>
@@ -119,6 +120,24 @@
   </si>
   <si>
     <t>Level 20 limit increase</t>
+  </si>
+  <si>
+    <t>Max strength attribute</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Might</t>
+  </si>
+  <si>
+    <t>Agility</t>
+  </si>
+  <si>
+    <t>Intelligence</t>
+  </si>
+  <si>
+    <t>Charisma</t>
   </si>
 </sst>
 </file>
@@ -181,11 +200,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,7 +543,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,38 +558,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -591,7 +610,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,22 +759,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6668388-8BB7-4E17-9B3D-DB53EBA3B344}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -779,159 +798,270 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>1</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="5">
-        <v>3</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="D3" s="4">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>5</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="5">
-        <v>7</v>
-      </c>
-      <c r="E5" s="5">
+      <c r="D5" s="4">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>10</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>13</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>15</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>18</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>20</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B60139-BDA5-4694-95B4-B5CCD376AFD6}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4">
+        <v>2</v>
+      </c>
+      <c r="G3" s="4">
+        <v>2</v>
+      </c>
+      <c r="H3" s="4">
+        <v>2</v>
+      </c>
+      <c r="I3" s="4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor: Modified test case for prime attribute to use a valid attribute selection based on the game rules (using standard array)
</commit_message>
<xml_diff>
--- a/DC20Models.nUnitTests/Unit Tests/Character/BlackBox_Character.xlsx
+++ b/DC20Models.nUnitTests/Unit Tests/Character/BlackBox_Character.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Blazor\DC20 Character Sheet\DC20Models\DC20Models.nUnitTests\Unit Tests\Character\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5502123-15FF-4004-9027-17F4CE4008B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B95070A-6E6D-4344-97FF-1451A70D1B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{4151E963-BEFA-4E14-B0A5-BD998C18A418}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="3" xr2:uid="{4151E963-BEFA-4E14-B0A5-BD998C18A418}"/>
   </bookViews>
   <sheets>
     <sheet name="Constructor" sheetId="2" r:id="rId1"/>
@@ -960,7 +960,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,13 +1041,13 @@
         <v>3</v>
       </c>
       <c r="F3" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="4">
         <v>2</v>
       </c>
       <c r="H3" s="4">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="I3" s="4">
         <v>3</v>

</xml_diff>

<commit_message>
Test: Create Health Point test case
</commit_message>
<xml_diff>
--- a/DC20Models.nUnitTests/Unit Tests/Character/BlackBox_Character.xlsx
+++ b/DC20Models.nUnitTests/Unit Tests/Character/BlackBox_Character.xlsx
@@ -8,15 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Blazor\DC20 Character Sheet\DC20Models\DC20Models.nUnitTests\Unit Tests\Character\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510F30A9-1907-4536-8268-83B154503F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D6C591-F823-4921-8BA2-378AF2B0E276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="3" xr2:uid="{4151E963-BEFA-4E14-B0A5-BD998C18A418}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="4" xr2:uid="{4151E963-BEFA-4E14-B0A5-BD998C18A418}"/>
   </bookViews>
   <sheets>
     <sheet name="Constructor" sheetId="2" r:id="rId1"/>
     <sheet name="CombatMastery" sheetId="1" r:id="rId2"/>
     <sheet name="AttributeLimit" sheetId="3" r:id="rId3"/>
     <sheet name="Prime" sheetId="4" r:id="rId4"/>
+    <sheet name="Health Points" sheetId="5" r:id="rId5"/>
+    <sheet name="Stamina Points" sheetId="6" r:id="rId6"/>
+    <sheet name="Mana Points" sheetId="7" r:id="rId7"/>
+    <sheet name="Physical Defense" sheetId="8" r:id="rId8"/>
+    <sheet name="Mental Defense" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="43">
   <si>
     <t>Test Case</t>
   </si>
@@ -150,6 +155,24 @@
   </si>
   <si>
     <t>Max Agility</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Ancestry</t>
+  </si>
+  <si>
+    <t>Martial Class</t>
+  </si>
+  <si>
+    <t>formula: 6 + Character Level + Might + Class + Ancestry</t>
+  </si>
+  <si>
+    <t>Commander</t>
+  </si>
+  <si>
+    <t>Human</t>
   </si>
 </sst>
 </file>
@@ -201,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -217,6 +240,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,7 +581,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,7 +798,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B60139-BDA5-4694-95B4-B5CCD376AFD6}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,4 +1218,480 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB43AFB8-132D-4E2B-BACC-B0D3E98F4493}">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="49.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4">
+        <v>2</v>
+      </c>
+      <c r="H3" s="4">
+        <v>-2</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="4">
+        <v>11</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="D1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{751A7B61-39A2-4577-B9E7-A4F6FB5CC004}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CC69D52-2D26-43B9-92DB-CA298B987AE1}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D7F92DA-ECF6-45EC-BF73-7A2A551F6FBE}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C0560B-4173-4695-BC24-36C0536370FD}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test: Add Health Point test case for Barbarian class
</commit_message>
<xml_diff>
--- a/DC20Models.nUnitTests/Unit Tests/Character/BlackBox_Character.xlsx
+++ b/DC20Models.nUnitTests/Unit Tests/Character/BlackBox_Character.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Blazor\DC20 Character Sheet\DC20Models\DC20Models.nUnitTests\Unit Tests\Character\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D6C591-F823-4921-8BA2-378AF2B0E276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F6166A-998B-40A8-8300-FAD94D5AA717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="4" xr2:uid="{4151E963-BEFA-4E14-B0A5-BD998C18A418}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{4151E963-BEFA-4E14-B0A5-BD998C18A418}"/>
   </bookViews>
   <sheets>
     <sheet name="Constructor" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="44">
   <si>
     <t>Test Case</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>Human</t>
+  </si>
+  <si>
+    <t>Barbarian</t>
   </si>
 </sst>
 </file>
@@ -1222,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB43AFB8-132D-4E2B-BACC-B0D3E98F4493}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,6 +1338,42 @@
       <c r="L3" s="6" t="s">
         <v>40</v>
       </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <v>2</v>
+      </c>
+      <c r="H4" s="4">
+        <v>-2</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="4">
+        <v>11</v>
+      </c>
+      <c r="L4" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Test: Added unit test Health Point value for Bard class.
</commit_message>
<xml_diff>
--- a/DC20Models.nUnitTests/Unit Tests/Character/BlackBox_Character.xlsx
+++ b/DC20Models.nUnitTests/Unit Tests/Character/BlackBox_Character.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Blazor\DC20 Character Sheet\DC20Models\DC20Models.nUnitTests\Unit Tests\Character\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F6166A-998B-40A8-8300-FAD94D5AA717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1253F9-34C3-482E-87E9-D3CC7DE0DD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{4151E963-BEFA-4E14-B0A5-BD998C18A418}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="44">
   <si>
     <t>Test Case</t>
   </si>
@@ -163,9 +163,6 @@
     <t>Ancestry</t>
   </si>
   <si>
-    <t>Martial Class</t>
-  </si>
-  <si>
     <t>formula: 6 + Character Level + Might + Class + Ancestry</t>
   </si>
   <si>
@@ -176,6 +173,9 @@
   </si>
   <si>
     <t>Barbarian</t>
+  </si>
+  <si>
+    <t>Bard</t>
   </si>
 </sst>
 </file>
@@ -1225,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB43AFB8-132D-4E2B-BACC-B0D3E98F4493}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,7 +1309,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -1327,16 +1327,16 @@
         <v>-2</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="K3" s="4">
         <v>11</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1347,7 +1347,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -1365,15 +1365,50 @@
         <v>-2</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K4" s="4">
         <v>11</v>
       </c>
       <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>-2</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="4">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>